<commit_message>
transport file missing UI
</commit_message>
<xml_diff>
--- a/Sifh.ReportGenerator/Excel Templates/Marumi.xlsx
+++ b/Sifh.ReportGenerator/Excel Templates/Marumi.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilherme\source\repos\brendongreene\Sifh.ReportGenerator\Sifh.ReportGenerator\Excel Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B525073-4158-40BA-9C96-8AD357FE8676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B98370-8AC6-4A5D-81C2-DB214FA420D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{997B08C3-0059-4A02-89AB-DD06527C47E4}"/>
+    <workbookView xWindow="7200" yWindow="1920" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{997B08C3-0059-4A02-89AB-DD06527C47E4}"/>
   </bookViews>
   <sheets>
     <sheet name="SVR" sheetId="6" r:id="rId1"/>
     <sheet name="FRR" sheetId="5" r:id="rId2"/>
+    <sheet name="TR" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="83">
   <si>
     <t>#31</t>
   </si>
@@ -215,13 +216,73 @@
   </si>
   <si>
     <t>LBS</t>
+  </si>
+  <si>
+    <t>SIFH GROUP TRANSPORT RECORD</t>
+  </si>
+  <si>
+    <t>Maurice Bishop International Airport</t>
+  </si>
+  <si>
+    <t>Finished Lot: 810 2023 0560</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Species</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Yellow fin Tuna</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CARGO INFORMATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Delivery Point</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Exit Point</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Transporter License/ Conductor License</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Truck License</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Transporter name/ Conductor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quantity of Boxes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cardboard/</t>
+  </si>
+  <si>
+    <t>Styrofoam</t>
+  </si>
+  <si>
+    <t>Net Weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Grand Mal St. George's</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cargo Handlers    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date                        </t>
+  </si>
+  <si>
+    <t>…..........................................................................................................</t>
+  </si>
+  <si>
+    <t>….........................................................................................................</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,6 +361,37 @@
       <name val="Calibri Light"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -309,7 +401,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -367,12 +459,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -396,6 +536,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -407,6 +566,45 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -988,10 +1186,10 @@
       <c r="I17" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="J17" s="19" t="s">
+      <c r="J17" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="K17" s="20"/>
+      <c r="K17" s="27"/>
       <c r="L17" s="13" t="s">
         <v>52</v>
       </c>
@@ -1022,10 +1220,10 @@
       <c r="I18" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J18" s="19" t="s">
+      <c r="J18" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="K18" s="20"/>
+      <c r="K18" s="27"/>
       <c r="L18" s="13" t="s">
         <v>17</v>
       </c>
@@ -1120,7 +1318,7 @@
   </sheetPr>
   <dimension ref="B8:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
@@ -1358,10 +1556,10 @@
       <c r="I20" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J20" s="21" t="s">
+      <c r="J20" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="K20" s="22"/>
+      <c r="K20" s="29"/>
       <c r="L20" s="6" t="s">
         <v>24</v>
       </c>
@@ -1388,10 +1586,10 @@
       <c r="I21" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J21" s="21" t="s">
+      <c r="J21" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="K21" s="22"/>
+      <c r="K21" s="29"/>
       <c r="L21" s="6" t="s">
         <v>16</v>
       </c>
@@ -1554,4 +1752,192 @@
   <pageSetup scale="66" orientation="landscape" r:id="rId2"/>
   <drawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A121C46-5236-4954-98A2-8B20B81722CE}">
+  <dimension ref="C4:H24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15:H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="6.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+    </row>
+    <row r="5" spans="3:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="31"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+    </row>
+    <row r="6" spans="3:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="31"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+    </row>
+    <row r="7" spans="3:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="31"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+    </row>
+    <row r="8" spans="3:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+    </row>
+    <row r="9" spans="3:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+    </row>
+    <row r="12" spans="3:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="33"/>
+      <c r="E12" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+    </row>
+    <row r="13" spans="3:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="H13" s="36"/>
+    </row>
+    <row r="14" spans="3:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="23"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" s="40"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="42"/>
+    </row>
+    <row r="15" spans="3:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="22"/>
+      <c r="E15" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+    </row>
+    <row r="23" spans="3:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="35"/>
+    </row>
+    <row r="24" spans="3:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="35"/>
+    </row>
+  </sheetData>
+  <mergeCells count="23">
+    <mergeCell ref="D23:H23"/>
+    <mergeCell ref="D24:H24"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update feb 6th 2024
</commit_message>
<xml_diff>
--- a/Sifh.ReportGenerator/Excel Templates/Marumi.xlsx
+++ b/Sifh.ReportGenerator/Excel Templates/Marumi.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilherme\Source\Repos\brendongreene\Sifh.ReportGenerator\Sifh.ReportGenerator\Excel Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilherme\source\repos\brendongreene\Sifh.ReportGenerator\Sifh.ReportGenerator\Excel Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971F977F-C3BD-4A8D-972D-BE268AF19AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB46CE47-4B53-40FA-AF25-0EB31378BF72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{997B08C3-0059-4A02-89AB-DD06527C47E4}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="82">
   <si>
     <t>#31</t>
   </si>
@@ -200,9 +200,6 @@
     <t>Delivery Port</t>
   </si>
   <si>
-    <t>ADRIAN BETHEL</t>
-  </si>
-  <si>
     <t xml:space="preserve">Captain </t>
   </si>
   <si>
@@ -224,9 +221,6 @@
     <t>Maurice Bishop International Airport</t>
   </si>
   <si>
-    <t>Finished Lot: 810 2023 0560</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Species</t>
   </si>
   <si>
@@ -276,6 +270,9 @@
   </si>
   <si>
     <t>….........................................................................................................</t>
+  </si>
+  <si>
+    <t>Finished Lot:</t>
   </si>
 </sst>
 </file>
@@ -512,7 +509,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -558,6 +555,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -603,7 +603,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1018,7 +1018,7 @@
   <dimension ref="B8:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,7 +1037,7 @@
   <sheetData>
     <row r="8" spans="2:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D8" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="1"/>
@@ -1048,7 +1048,7 @@
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>16</v>
@@ -1066,7 +1066,7 @@
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>12</v>
@@ -1084,11 +1084,9 @@
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" s="15" t="s">
         <v>57</v>
       </c>
+      <c r="C12" s="15"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -1189,10 +1187,10 @@
       <c r="I17" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="J17" s="27" t="s">
+      <c r="J17" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="K17" s="28"/>
+      <c r="K17" s="29"/>
       <c r="L17" s="13" t="s">
         <v>52</v>
       </c>
@@ -1223,10 +1221,10 @@
       <c r="I18" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J18" s="27" t="s">
+      <c r="J18" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="K18" s="28"/>
+      <c r="K18" s="29"/>
       <c r="L18" s="13" t="s">
         <v>17</v>
       </c>
@@ -1259,7 +1257,7 @@
       </c>
       <c r="J19" s="17"/>
       <c r="K19" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L19" s="12"/>
       <c r="M19" s="1"/>
@@ -1322,7 +1320,7 @@
   <dimension ref="B8:M36"/>
   <sheetViews>
     <sheetView view="pageLayout" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1559,10 +1557,10 @@
       <c r="I20" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J20" s="29" t="s">
+      <c r="J20" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="K20" s="30"/>
+      <c r="K20" s="31"/>
       <c r="L20" s="6" t="s">
         <v>24</v>
       </c>
@@ -1589,10 +1587,10 @@
       <c r="I21" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J21" s="29" t="s">
+      <c r="J21" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="K21" s="30"/>
+      <c r="K21" s="31"/>
       <c r="L21" s="6" t="s">
         <v>16</v>
       </c>
@@ -1623,7 +1621,7 @@
       </c>
       <c r="J22" s="18"/>
       <c r="K22" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L22" s="3"/>
       <c r="M22" s="1"/>
@@ -1761,8 +1759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A121C46-5236-4954-98A2-8B20B81722CE}">
   <dimension ref="C4:H24"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1770,153 +1768,153 @@
     <col min="2" max="2" width="6.42578125" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
     <col min="4" max="4" width="22.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
     <col min="6" max="6" width="8.85546875" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" customWidth="1"/>
     <col min="8" max="8" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="43" t="s">
+      <c r="C4" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+    </row>
+    <row r="5" spans="3:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="42"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+    </row>
+    <row r="6" spans="3:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="42"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+    </row>
+    <row r="7" spans="3:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="42"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+    </row>
+    <row r="8" spans="3:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+    </row>
+    <row r="9" spans="3:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-    </row>
-    <row r="5" spans="3:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-    </row>
-    <row r="6" spans="3:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="41" t="s">
-        <v>72</v>
-      </c>
-      <c r="D6" s="41"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-    </row>
-    <row r="7" spans="3:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="41" t="s">
-        <v>71</v>
-      </c>
-      <c r="D7" s="41"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-    </row>
-    <row r="8" spans="3:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41" t="s">
-        <v>78</v>
-      </c>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-    </row>
-    <row r="9" spans="3:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="41" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
     </row>
     <row r="12" spans="3:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
+      <c r="C12" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="40"/>
+      <c r="E12" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
     </row>
     <row r="13" spans="3:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="E13" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="H13" s="32"/>
+      <c r="H13" s="33"/>
     </row>
     <row r="14" spans="3:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="23"/>
       <c r="D14" s="24"/>
-      <c r="E14" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="F14" s="36"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="38"/>
+      <c r="E14" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="F14" s="37"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="39"/>
     </row>
     <row r="15" spans="3:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D15" s="22"/>
-      <c r="E15" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="F15" s="33"/>
+      <c r="E15" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" s="34"/>
       <c r="G15" s="26"/>
       <c r="H15" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
     </row>
     <row r="23" spans="3:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C23" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="D23" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="E23" s="31"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
     </row>
     <row r="24" spans="3:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="D24" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="22">
@@ -1931,8 +1929,8 @@
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="E9:H9"/>
     <mergeCell ref="E8:H8"/>
-    <mergeCell ref="E12:H12"/>
     <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F12:H12"/>
     <mergeCell ref="D23:H23"/>
     <mergeCell ref="D24:H24"/>
     <mergeCell ref="G13:H13"/>

</xml_diff>